<commit_message>
Corrigindo erro de Lógica NRU
</commit_message>
<xml_diff>
--- a/Tabelas para o relatório.xlsx
+++ b/Tabelas para o relatório.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Plufty\Desktop\5º Período\Sistemas Operacionais\Projeto\Algoritimos Memoria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B0EA11-F18C-4B6A-9871-DC36C25A2875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699AE47B-7529-4DE2-A639-C7C1156C47C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5D7EFB73-A786-4432-A134-C272E8088DB6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5D7EFB73-A786-4432-A134-C272E8088DB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -111,7 +111,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -134,11 +134,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -149,6 +160,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,34 +423,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>11</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1034,34 +1046,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1657,34 +1669,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2843,34 +2855,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2912,34 +2924,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3535,34 +3547,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7691,8 +7703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE71603F-D43C-47F5-A0DE-AC867211C97C}">
   <dimension ref="Q1:AF79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Z57" sqref="Z57"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AE10" sqref="AE10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7773,7 +7785,7 @@
         <v>12</v>
       </c>
       <c r="T3" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="U3" s="1">
         <v>9</v>
@@ -7817,7 +7829,7 @@
         <v>12</v>
       </c>
       <c r="T4" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="U4" s="1">
         <v>9</v>
@@ -7857,7 +7869,7 @@
         <v>12</v>
       </c>
       <c r="T5" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="U5" s="1">
         <v>9</v>
@@ -7897,7 +7909,7 @@
         <v>12</v>
       </c>
       <c r="T6" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="U6" s="1">
         <v>9</v>
@@ -7937,7 +7949,7 @@
         <v>12</v>
       </c>
       <c r="T7" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="U7" s="1">
         <v>9</v>
@@ -7977,7 +7989,7 @@
         <v>12</v>
       </c>
       <c r="T8" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="U8" s="1">
         <v>9</v>
@@ -8017,7 +8029,7 @@
         <v>12</v>
       </c>
       <c r="T9" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="U9" s="1">
         <v>9</v>
@@ -8057,7 +8069,7 @@
         <v>12</v>
       </c>
       <c r="T10" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="U10" s="1">
         <v>9</v>
@@ -8097,7 +8109,7 @@
         <v>12</v>
       </c>
       <c r="T11" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="U11" s="1">
         <v>9</v>
@@ -8137,7 +8149,7 @@
         <v>12</v>
       </c>
       <c r="T12" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="U12" s="1">
         <v>9</v>
@@ -8233,10 +8245,10 @@
         <v>9</v>
       </c>
       <c r="Z16" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AA16" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AB16" s="1">
         <v>7</v>
@@ -8259,7 +8271,7 @@
         <v>9</v>
       </c>
       <c r="T17" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="U17" s="1">
         <v>7</v>
@@ -8277,10 +8289,10 @@
         <v>9</v>
       </c>
       <c r="Z17" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AA17" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AB17" s="1">
         <v>7</v>
@@ -8301,7 +8313,7 @@
         <v>9</v>
       </c>
       <c r="T18" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="U18" s="1">
         <v>7</v>
@@ -8317,10 +8329,10 @@
         <v>9</v>
       </c>
       <c r="Z18" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AA18" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AB18" s="1">
         <v>7</v>
@@ -8341,7 +8353,7 @@
         <v>9</v>
       </c>
       <c r="T19" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="U19" s="1">
         <v>7</v>
@@ -8357,10 +8369,10 @@
         <v>9</v>
       </c>
       <c r="Z19" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AA19" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AB19" s="1">
         <v>7</v>
@@ -8381,7 +8393,7 @@
         <v>9</v>
       </c>
       <c r="T20" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="U20" s="1">
         <v>7</v>
@@ -8397,10 +8409,10 @@
         <v>9</v>
       </c>
       <c r="Z20" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AA20" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AB20" s="1">
         <v>7</v>
@@ -8421,7 +8433,7 @@
         <v>9</v>
       </c>
       <c r="T21" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="U21" s="1">
         <v>7</v>
@@ -8437,10 +8449,10 @@
         <v>9</v>
       </c>
       <c r="Z21" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AA21" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AB21" s="1">
         <v>7</v>
@@ -8461,7 +8473,7 @@
         <v>9</v>
       </c>
       <c r="T22" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="U22" s="1">
         <v>7</v>
@@ -8477,10 +8489,10 @@
         <v>9</v>
       </c>
       <c r="Z22" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AA22" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AB22" s="1">
         <v>7</v>
@@ -8501,7 +8513,7 @@
         <v>9</v>
       </c>
       <c r="T23" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="U23" s="1">
         <v>7</v>
@@ -8517,10 +8529,10 @@
         <v>9</v>
       </c>
       <c r="Z23" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AA23" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AB23" s="1">
         <v>7</v>
@@ -8541,7 +8553,7 @@
         <v>9</v>
       </c>
       <c r="T24" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="U24" s="1">
         <v>7</v>
@@ -8557,10 +8569,10 @@
         <v>9</v>
       </c>
       <c r="Z24" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AA24" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AB24" s="1">
         <v>7</v>
@@ -8581,7 +8593,7 @@
         <v>9</v>
       </c>
       <c r="T25" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="U25" s="1">
         <v>7</v>
@@ -8597,10 +8609,10 @@
         <v>9</v>
       </c>
       <c r="Z25" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AA25" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AB25" s="1">
         <v>7</v>
@@ -8621,7 +8633,7 @@
         <v>9</v>
       </c>
       <c r="T26" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="U26" s="1">
         <v>7</v>
@@ -8699,7 +8711,7 @@
         <v>10</v>
       </c>
       <c r="T30" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U30" s="1">
         <v>6</v>
@@ -8720,7 +8732,7 @@
         <v>10</v>
       </c>
       <c r="AA30" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AB30" s="1">
         <v>6</v>
@@ -8743,7 +8755,7 @@
         <v>10</v>
       </c>
       <c r="T31" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U31" s="1">
         <v>6</v>
@@ -8762,7 +8774,7 @@
         <v>10</v>
       </c>
       <c r="AA31" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AB31" s="1">
         <v>6</v>
@@ -8783,7 +8795,7 @@
         <v>10</v>
       </c>
       <c r="T32" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U32" s="1">
         <v>6</v>
@@ -8802,7 +8814,7 @@
         <v>10</v>
       </c>
       <c r="AA32" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AB32" s="1">
         <v>6</v>
@@ -8823,7 +8835,7 @@
         <v>10</v>
       </c>
       <c r="T33" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U33" s="1">
         <v>6</v>
@@ -8842,7 +8854,7 @@
         <v>10</v>
       </c>
       <c r="AA33" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AB33" s="1">
         <v>6</v>
@@ -8863,7 +8875,7 @@
         <v>10</v>
       </c>
       <c r="T34" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U34" s="1">
         <v>6</v>
@@ -8882,7 +8894,7 @@
         <v>10</v>
       </c>
       <c r="AA34" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AB34" s="1">
         <v>6</v>
@@ -8903,7 +8915,7 @@
         <v>10</v>
       </c>
       <c r="T35" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U35" s="1">
         <v>6</v>
@@ -8922,7 +8934,7 @@
         <v>10</v>
       </c>
       <c r="AA35" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AB35" s="1">
         <v>6</v>
@@ -8943,7 +8955,7 @@
         <v>10</v>
       </c>
       <c r="T36" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U36" s="1">
         <v>6</v>
@@ -8962,7 +8974,7 @@
         <v>10</v>
       </c>
       <c r="AA36" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AB36" s="1">
         <v>6</v>
@@ -8983,7 +8995,7 @@
         <v>10</v>
       </c>
       <c r="T37" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U37" s="1">
         <v>6</v>
@@ -9002,7 +9014,7 @@
         <v>10</v>
       </c>
       <c r="AA37" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AB37" s="1">
         <v>6</v>
@@ -9023,7 +9035,7 @@
         <v>10</v>
       </c>
       <c r="T38" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U38" s="1">
         <v>6</v>
@@ -9042,7 +9054,7 @@
         <v>10</v>
       </c>
       <c r="AA38" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AB38" s="1">
         <v>6</v>
@@ -9063,7 +9075,7 @@
         <v>10</v>
       </c>
       <c r="T39" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U39" s="1">
         <v>6</v>
@@ -9082,7 +9094,7 @@
         <v>10</v>
       </c>
       <c r="AA39" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AB39" s="1">
         <v>6</v>
@@ -9091,6 +9103,9 @@
         <v>6</v>
       </c>
       <c r="AD39" s="4"/>
+    </row>
+    <row r="40" spans="17:30" x14ac:dyDescent="0.25">
+      <c r="T40" s="6"/>
     </row>
     <row r="53" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="79" spans="32:32" x14ac:dyDescent="0.25">

</xml_diff>